<commit_message>
hopefully addressed Shantenu's remarks
git-svn-id: file://localhost/tmp/svn2git/svn@2953 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/cloudcom10/performance/namd_runs.xlsx
+++ b/papers/cloudcom10/performance/namd_runs.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="252">
   <si>
     <t>SAGA Pilot Sub-Job Runtime</t>
     <phoneticPr fontId="17" type="noConversion"/>
@@ -75,7 +75,6 @@
   </si>
   <si>
     <t>large</t>
-    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>large</t>
@@ -2668,19 +2667,19 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.05865647261111</c:v>
+                  <c:v>36.77484585247222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.09388968944445</c:v>
+                  <c:v>36.7542692002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.45077452958333</c:v>
+                  <c:v>36.43405471177778</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.34425558349999</c:v>
+                  <c:v>37.77104676233333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.32852852341667</c:v>
+                  <c:v>38.53255338933333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12817,7 +12816,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
@@ -13317,7 +13315,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -13558,7 +13555,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -13571,11 +13567,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43:M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -14392,23 +14388,23 @@
         <v>18</v>
       </c>
       <c r="J36" s="76">
-        <f>AVERAGE(E145:E147)/60</f>
+        <f>AVERAGE(E155:E157)/60</f>
         <v>85.873793250944431</v>
       </c>
       <c r="K36" s="76">
-        <f>AVERAGE(E148:E150)/60</f>
+        <f>AVERAGE(E158:E160)/60</f>
         <v>86.0579628335</v>
       </c>
       <c r="L36" s="76">
-        <f>AVERAGE(E154:E156)/60</f>
+        <f>AVERAGE(E164:E166)/60</f>
         <v>86.760683253111111</v>
       </c>
       <c r="M36" s="76">
-        <f>AVERAGE(E154:E156)/60</f>
+        <f>AVERAGE(E164:E166)/60</f>
         <v>86.760683253111111</v>
       </c>
       <c r="N36" s="76">
-        <f>AVERAGE(E157:E158)/60</f>
+        <f>AVERAGE(E167:E168)/60</f>
         <v>90.030957966666662</v>
       </c>
       <c r="O36" s="76">
@@ -14502,36 +14498,36 @@
         <v>22</v>
       </c>
       <c r="J38" s="76">
-        <f>AVERAGE(E60:E62)/60</f>
-        <v>36.058656472611112</v>
+        <f>AVERAGE(E60:E65)/60</f>
+        <v>36.774845852472218</v>
       </c>
       <c r="K38" s="76">
-        <f>AVERAGE(E63:E65)/60</f>
-        <v>37.093889689444445</v>
+        <f>AVERAGE(E66:E70)/60</f>
+        <v>36.7542692002</v>
       </c>
       <c r="L38" s="76">
-        <f>AVERAGE(E66:E69)/60</f>
-        <v>38.450774529583327</v>
+        <f>AVERAGE(E71:E76)/60</f>
+        <v>36.434054711777776</v>
       </c>
       <c r="M38" s="76">
-        <f>AVERAGE(E70:E73)/60</f>
-        <v>39.344255583499994</v>
+        <f>AVERAGE(E77:E82)/60</f>
+        <v>37.771046762333334</v>
       </c>
       <c r="N38" s="76">
-        <f>AVERAGE(E74:E75)/60</f>
-        <v>39.328528523416665</v>
+        <f>AVERAGE(E83:E85)/60</f>
+        <v>38.53255338933333</v>
       </c>
       <c r="O38" s="76">
         <f>AVERAGE(J38:N38)</f>
-        <v>38.055220959711107</v>
+        <v>37.253353983223327</v>
       </c>
       <c r="P38">
         <f t="shared" si="1"/>
-        <v>2.288695582760528</v>
+        <v>2.337959050631786</v>
       </c>
       <c r="Q38">
         <f>P38/4</f>
-        <v>0.572173895690132</v>
+        <v>0.5844897626579465</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -14557,23 +14553,23 @@
         <v>24</v>
       </c>
       <c r="J39" s="76">
-        <f>AVERAGE(E76:E92)/60</f>
+        <f>AVERAGE(E86:E102)/60</f>
         <v>29.755726918294116</v>
       </c>
       <c r="K39" s="76">
-        <f>AVERAGE(E98:E100)/60</f>
+        <f>AVERAGE(E108:E110)/60</f>
         <v>29.533525637777775</v>
       </c>
       <c r="L39" s="76">
-        <f>AVERAGE(E109:E125)/60</f>
+        <f>AVERAGE(E119:E135)/60</f>
         <v>30.22606411610785</v>
       </c>
       <c r="M39" s="76">
-        <f>AVERAGE(E126:E130)/60</f>
+        <f>AVERAGE(E136:E140)/60</f>
         <v>29.968669529766665</v>
       </c>
       <c r="N39" s="76">
-        <f>AVERAGE(E135:E136)/60</f>
+        <f>AVERAGE(E145:E146)/60</f>
         <v>28.153145275583331</v>
       </c>
       <c r="O39" s="76">
@@ -14648,21 +14644,6 @@
       <c r="F42" t="s">
         <v>175</v>
       </c>
-      <c r="I42" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" t="s">
-        <v>21</v>
-      </c>
-      <c r="M42" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" t="s">
@@ -14683,20 +14664,20 @@
       <c r="F43" t="s">
         <v>175</v>
       </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
-      <c r="J43" s="76">
-        <v>90.772995064666674</v>
-      </c>
-      <c r="K43" s="76">
-        <v>54.981918734250002</v>
-      </c>
-      <c r="L43" s="76">
-        <v>36.058656472611112</v>
-      </c>
-      <c r="M43" s="76">
-        <v>29.755726918294116</v>
+      <c r="I43" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -14719,19 +14700,19 @@
         <v>175</v>
       </c>
       <c r="I44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J44" s="76">
-        <v>90.256347600583325</v>
+        <v>85.873793250944431</v>
       </c>
       <c r="K44" s="76">
-        <v>55.322307368083329</v>
+        <v>53.555982869466668</v>
       </c>
       <c r="L44" s="76">
-        <v>37.093889689444445</v>
+        <v>36.774845852472218</v>
       </c>
       <c r="M44" s="76">
-        <v>29.533525637777775</v>
+        <v>29.755726918294116</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -14754,19 +14735,19 @@
         <v>175</v>
       </c>
       <c r="I45">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J45" s="76">
-        <v>91.132208150583338</v>
+        <v>86.0579628335</v>
       </c>
       <c r="K45" s="76">
-        <v>56.079986642444439</v>
+        <v>53.937479001249997</v>
       </c>
       <c r="L45" s="76">
-        <v>38.450774529583327</v>
+        <v>36.7542692002</v>
       </c>
       <c r="M45" s="76">
-        <v>30.22606411610785</v>
+        <v>29.533525637777775</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -14789,19 +14770,19 @@
         <v>175</v>
       </c>
       <c r="I46">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J46" s="76">
-        <v>95.949001352933323</v>
+        <v>86.760683253111111</v>
       </c>
       <c r="K46" s="76">
-        <v>55.409327467277784</v>
+        <v>54.959793672277776</v>
       </c>
       <c r="L46" s="76">
-        <v>39.344255583499994</v>
+        <v>36.434054711777776</v>
       </c>
       <c r="M46" s="76">
-        <v>29.968669529766665</v>
+        <v>30.22606411610785</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -14824,19 +14805,19 @@
         <v>175</v>
       </c>
       <c r="I47">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J47" s="76">
-        <v>93.94475276866666</v>
+        <v>86.760683253111111</v>
       </c>
       <c r="K47" s="76">
-        <v>56.714765632166667</v>
+        <v>54.435406076111114</v>
       </c>
       <c r="L47" s="76">
-        <v>39.328528523416665</v>
+        <v>37.771046762333334</v>
       </c>
       <c r="M47" s="76">
-        <v>28.153145275583331</v>
+        <v>29.968669529766665</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -14858,6 +14839,21 @@
       <c r="F48" t="s">
         <v>175</v>
       </c>
+      <c r="I48">
+        <v>32</v>
+      </c>
+      <c r="J48" s="76">
+        <v>90.030957966666662</v>
+      </c>
+      <c r="K48" s="76">
+        <v>57.030591033333344</v>
+      </c>
+      <c r="L48" s="76">
+        <v>38.53255338933333</v>
+      </c>
+      <c r="M48" s="76">
+        <v>28.153145275583331</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
@@ -15081,7 +15077,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60" s="74">
         <v>4</v>
@@ -15093,15 +15089,15 @@
         <v>4</v>
       </c>
       <c r="E60" s="82">
-        <v>2062.0451450300002</v>
-      </c>
-      <c r="F60" s="74" t="s">
+        <v>2165.2144379599999</v>
+      </c>
+      <c r="F60" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61" s="74">
         <v>4</v>
@@ -15113,15 +15109,15 @@
         <v>4</v>
       </c>
       <c r="E61" s="82">
-        <v>2197.8351230600001</v>
-      </c>
-      <c r="F61" s="74" t="s">
+        <v>2283.2516999200002</v>
+      </c>
+      <c r="F61" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62" s="74">
         <v>4</v>
@@ -15133,69 +15129,69 @@
         <v>4</v>
       </c>
       <c r="E62" s="82">
-        <v>2230.6778969799998</v>
-      </c>
-      <c r="F62" s="74" t="s">
+        <v>2173.3167338399999</v>
+      </c>
+      <c r="F62" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63" s="74">
         <v>4</v>
       </c>
       <c r="C63" s="74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D63" s="74">
         <v>4</v>
       </c>
       <c r="E63" s="82">
-        <v>2214.5342040099999</v>
-      </c>
-      <c r="F63" s="74" t="s">
+        <v>2185.1247549099999</v>
+      </c>
+      <c r="F63" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B64" s="74">
         <v>4</v>
       </c>
       <c r="C64" s="74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D64" s="74">
         <v>4</v>
       </c>
       <c r="E64" s="82">
-        <v>2227.3965690099999</v>
-      </c>
-      <c r="F64" s="74" t="s">
+        <v>2269.9999311000001</v>
+      </c>
+      <c r="F64" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B65" s="74">
         <v>4</v>
       </c>
       <c r="C65" s="74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D65" s="74">
         <v>4</v>
       </c>
       <c r="E65" s="82">
-        <v>2234.9693710800002</v>
-      </c>
-      <c r="F65" s="74" t="s">
+        <v>2162.0369491599999</v>
+      </c>
+      <c r="F65" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15207,15 +15203,15 @@
         <v>4</v>
       </c>
       <c r="C66" s="74">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D66" s="74">
         <v>4</v>
       </c>
       <c r="E66" s="82">
-        <v>2318.40899515</v>
-      </c>
-      <c r="F66" s="74" t="s">
+        <v>2319.98405099</v>
+      </c>
+      <c r="F66" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15227,15 +15223,15 @@
         <v>4</v>
       </c>
       <c r="C67" s="74">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D67" s="74">
         <v>4</v>
       </c>
       <c r="E67" s="82">
-        <v>2381.80929685</v>
-      </c>
-      <c r="F67" s="74" t="s">
+        <v>2165.4693579700001</v>
+      </c>
+      <c r="F67" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15247,15 +15243,15 @@
         <v>4</v>
       </c>
       <c r="C68" s="74">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D68" s="74">
         <v>4</v>
       </c>
       <c r="E68" s="82">
-        <v>2220.3577370600001</v>
-      </c>
-      <c r="F68" s="74" t="s">
+        <v>2171.7986049699998</v>
+      </c>
+      <c r="F68" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15267,15 +15263,15 @@
         <v>4</v>
       </c>
       <c r="C69" s="74">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D69" s="74">
         <v>4</v>
       </c>
       <c r="E69" s="82">
-        <v>2307.6098580399998</v>
-      </c>
-      <c r="F69" s="74" t="s">
+        <v>2183.7792851899999</v>
+      </c>
+      <c r="F69" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15287,15 +15283,15 @@
         <v>4</v>
       </c>
       <c r="C70" s="74">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D70" s="74">
         <v>4</v>
       </c>
       <c r="E70" s="82">
-        <v>2470.72962117</v>
-      </c>
-      <c r="F70" s="74" t="s">
+        <v>2185.2494609400001</v>
+      </c>
+      <c r="F70" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15307,15 +15303,15 @@
         <v>4</v>
       </c>
       <c r="C71" s="74">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D71" s="74">
         <v>4</v>
       </c>
       <c r="E71" s="82">
-        <v>2315.60190797</v>
-      </c>
-      <c r="F71" s="74" t="s">
+        <v>2137.2723250399999</v>
+      </c>
+      <c r="F71" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15327,15 +15323,15 @@
         <v>4</v>
       </c>
       <c r="C72" s="74">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D72" s="74">
         <v>4</v>
       </c>
       <c r="E72" s="82">
-        <v>2394.6190059199998</v>
-      </c>
-      <c r="F72" s="74" t="s">
+        <v>2220.7439541799999</v>
+      </c>
+      <c r="F72" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15347,35 +15343,35 @@
         <v>4</v>
       </c>
       <c r="C73" s="74">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D73" s="74">
         <v>4</v>
       </c>
       <c r="E73" s="82">
-        <v>2261.67080498</v>
-      </c>
-      <c r="F73" s="74" t="s">
+        <v>2110.8885998699998</v>
+      </c>
+      <c r="F73" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B74" s="74">
         <v>4</v>
       </c>
       <c r="C74" s="74">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D74" s="74">
         <v>4</v>
       </c>
       <c r="E74" s="82">
-        <v>2428.40984893</v>
-      </c>
-      <c r="F74" s="74" t="s">
+        <v>2212.8257401000001</v>
+      </c>
+      <c r="F74" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15387,215 +15383,215 @@
         <v>4</v>
       </c>
       <c r="C75" s="74">
+        <v>8</v>
+      </c>
+      <c r="D75" s="74">
+        <v>4</v>
+      </c>
+      <c r="E75" s="82">
+        <v>2209.1583819399998</v>
+      </c>
+      <c r="F75" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" s="74">
+        <v>4</v>
+      </c>
+      <c r="C76" s="74">
+        <v>8</v>
+      </c>
+      <c r="D76" s="74">
+        <v>4</v>
+      </c>
+      <c r="E76" s="82">
+        <v>2225.3706951099998</v>
+      </c>
+      <c r="F76" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" s="74">
+        <v>4</v>
+      </c>
+      <c r="C77" s="74">
+        <v>16</v>
+      </c>
+      <c r="D77" s="74">
+        <v>4</v>
+      </c>
+      <c r="E77" s="82">
+        <v>2225.0072731999999</v>
+      </c>
+      <c r="F77" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" s="74">
+        <v>4</v>
+      </c>
+      <c r="C78" s="74">
+        <v>16</v>
+      </c>
+      <c r="D78" s="74">
+        <v>4</v>
+      </c>
+      <c r="E78" s="82">
+        <v>2296.1518640499999</v>
+      </c>
+      <c r="F78" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="74">
+        <v>4</v>
+      </c>
+      <c r="C79" s="74">
+        <v>16</v>
+      </c>
+      <c r="D79" s="74">
+        <v>4</v>
+      </c>
+      <c r="E79" s="82">
+        <v>2285.0504000199999</v>
+      </c>
+      <c r="F79" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="74">
+        <v>4</v>
+      </c>
+      <c r="C80" s="74">
+        <v>16</v>
+      </c>
+      <c r="D80" s="74">
+        <v>4</v>
+      </c>
+      <c r="E80" s="82">
+        <v>2199.4940891299998</v>
+      </c>
+      <c r="F80" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="74">
+        <v>4</v>
+      </c>
+      <c r="C81" s="74">
+        <v>16</v>
+      </c>
+      <c r="D81" s="74">
+        <v>4</v>
+      </c>
+      <c r="E81" s="82">
+        <v>2291.9013450100001</v>
+      </c>
+      <c r="F81" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="74">
+        <v>4</v>
+      </c>
+      <c r="C82" s="74">
+        <v>16</v>
+      </c>
+      <c r="D82" s="74">
+        <v>4</v>
+      </c>
+      <c r="E82" s="82">
+        <v>2299.9718630299999</v>
+      </c>
+      <c r="F82" s="82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" s="74">
+        <v>4</v>
+      </c>
+      <c r="C83" s="74">
         <v>32</v>
       </c>
-      <c r="D75" s="74">
-        <v>4</v>
-      </c>
-      <c r="E75" s="82">
-        <v>2291.01357388</v>
-      </c>
-      <c r="F75" s="74" t="s">
+      <c r="D83" s="74">
+        <v>4</v>
+      </c>
+      <c r="E83" s="82">
+        <v>2319.8565950399998</v>
+      </c>
+      <c r="F83" s="82" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
-        <v>177</v>
-      </c>
-      <c r="B76">
-        <v>8</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76">
-        <v>4</v>
-      </c>
-      <c r="E76" s="81">
-        <v>1755.41372609</v>
-      </c>
-      <c r="F76" t="s">
+    <row r="84" spans="1:6">
+      <c r="A84" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" s="74">
+        <v>4</v>
+      </c>
+      <c r="C84" s="74">
+        <v>32</v>
+      </c>
+      <c r="D84" s="74">
+        <v>4</v>
+      </c>
+      <c r="E84" s="82">
+        <v>2326.5095250600002</v>
+      </c>
+      <c r="F84" s="82" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>177</v>
-      </c>
-      <c r="B77">
-        <v>8</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77">
-        <v>4</v>
-      </c>
-      <c r="E77" s="81">
-        <v>1700.6529159500001</v>
-      </c>
-      <c r="F77" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
-        <v>177</v>
-      </c>
-      <c r="B78">
-        <v>8</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
-        <v>4</v>
-      </c>
-      <c r="E78" s="81">
-        <v>1791.71858215</v>
-      </c>
-      <c r="F78" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>177</v>
-      </c>
-      <c r="B79">
-        <v>8</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79">
-        <v>4</v>
-      </c>
-      <c r="E79" s="81">
-        <v>1754.3026611800001</v>
-      </c>
-      <c r="F79" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" t="s">
-        <v>177</v>
-      </c>
-      <c r="B80">
-        <v>8</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80">
-        <v>4</v>
-      </c>
-      <c r="E80" s="81">
-        <v>1795.45695019</v>
-      </c>
-      <c r="F80" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" t="s">
-        <v>177</v>
-      </c>
-      <c r="B81">
-        <v>8</v>
-      </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81">
-        <v>4</v>
-      </c>
-      <c r="E81" s="81">
-        <v>1768.0575780900001</v>
-      </c>
-      <c r="F81" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" t="s">
-        <v>177</v>
-      </c>
-      <c r="B82">
-        <v>8</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82">
-        <v>4</v>
-      </c>
-      <c r="E82" s="81">
-        <v>1768.25146008</v>
-      </c>
-      <c r="F82" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" t="s">
-        <v>177</v>
-      </c>
-      <c r="B83">
-        <v>8</v>
-      </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-      <c r="D83">
-        <v>4</v>
-      </c>
-      <c r="E83" s="81">
-        <v>1872.71734595</v>
-      </c>
-      <c r="F83" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" t="s">
-        <v>177</v>
-      </c>
-      <c r="B84">
-        <v>8</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-      <c r="D84">
-        <v>4</v>
-      </c>
-      <c r="E84" s="81">
-        <v>1780.7754190000001</v>
-      </c>
-      <c r="F84" t="s">
-        <v>175</v>
-      </c>
-    </row>
     <row r="85" spans="1:6">
-      <c r="A85" t="s">
-        <v>177</v>
-      </c>
-      <c r="B85">
-        <v>8</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85">
-        <v>4</v>
-      </c>
-      <c r="E85" s="81">
-        <v>1772.9535300699999</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="A85" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" s="74">
+        <v>4</v>
+      </c>
+      <c r="C85" s="74">
+        <v>32</v>
+      </c>
+      <c r="D85" s="74">
+        <v>4</v>
+      </c>
+      <c r="E85" s="82">
+        <v>2289.49348998</v>
+      </c>
+      <c r="F85" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -15613,7 +15609,7 @@
         <v>4</v>
       </c>
       <c r="E86" s="81">
-        <v>1673.50027084</v>
+        <v>1755.41372609</v>
       </c>
       <c r="F86" t="s">
         <v>175</v>
@@ -15633,7 +15629,7 @@
         <v>4</v>
       </c>
       <c r="E87" s="81">
-        <v>1788.05790305</v>
+        <v>1700.6529159500001</v>
       </c>
       <c r="F87" t="s">
         <v>175</v>
@@ -15653,7 +15649,7 @@
         <v>4</v>
       </c>
       <c r="E88" s="81">
-        <v>1892.5188911</v>
+        <v>1791.71858215</v>
       </c>
       <c r="F88" t="s">
         <v>175</v>
@@ -15673,7 +15669,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="81">
-        <v>1890.1004610099999</v>
+        <v>1754.3026611800001</v>
       </c>
       <c r="F89" t="s">
         <v>175</v>
@@ -15693,7 +15689,7 @@
         <v>4</v>
       </c>
       <c r="E90" s="81">
-        <v>1800.52480197</v>
+        <v>1795.45695019</v>
       </c>
       <c r="F90" t="s">
         <v>175</v>
@@ -15713,7 +15709,7 @@
         <v>4</v>
       </c>
       <c r="E91" s="81">
-        <v>1778.2094800499999</v>
+        <v>1768.0575780900001</v>
       </c>
       <c r="F91" t="s">
         <v>175</v>
@@ -15733,7 +15729,7 @@
         <v>4</v>
       </c>
       <c r="E92" s="81">
-        <v>1767.6294798900001</v>
+        <v>1768.25146008</v>
       </c>
       <c r="F92" t="s">
         <v>175</v>
@@ -15753,7 +15749,10 @@
         <v>4</v>
       </c>
       <c r="E93" s="81">
-        <v>1755.7615511399999</v>
+        <v>1872.71734595</v>
+      </c>
+      <c r="F93" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -15770,7 +15769,10 @@
         <v>4</v>
       </c>
       <c r="E94" s="81">
-        <v>1755.3108708899999</v>
+        <v>1780.7754190000001</v>
+      </c>
+      <c r="F94" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -15787,7 +15789,10 @@
         <v>4</v>
       </c>
       <c r="E95" s="81">
-        <v>1776.3025808299999</v>
+        <v>1772.9535300699999</v>
+      </c>
+      <c r="F95" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -15804,7 +15809,10 @@
         <v>4</v>
       </c>
       <c r="E96" s="81">
-        <v>1775.4375519800001</v>
+        <v>1673.50027084</v>
+      </c>
+      <c r="F96" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -15821,7 +15829,10 @@
         <v>4</v>
       </c>
       <c r="E97" s="81">
-        <v>1771.63202095</v>
+        <v>1788.05790305</v>
+      </c>
+      <c r="F97" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -15832,13 +15843,13 @@
         <v>8</v>
       </c>
       <c r="C98">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D98">
         <v>4</v>
       </c>
       <c r="E98" s="81">
-        <v>1727.25121689</v>
+        <v>1892.5188911</v>
       </c>
       <c r="F98" t="s">
         <v>175</v>
@@ -15852,13 +15863,13 @@
         <v>8</v>
       </c>
       <c r="C99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D99">
         <v>4</v>
       </c>
       <c r="E99" s="81">
-        <v>1818.3420629499999</v>
+        <v>1890.1004610099999</v>
       </c>
       <c r="F99" t="s">
         <v>175</v>
@@ -15872,13 +15883,13 @@
         <v>8</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
       <c r="E100" s="81">
-        <v>1770.4413349599999</v>
+        <v>1800.52480197</v>
       </c>
       <c r="F100" t="s">
         <v>175</v>
@@ -15892,13 +15903,13 @@
         <v>8</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D101">
         <v>4</v>
       </c>
       <c r="E101" s="81">
-        <v>1894.0333972000001</v>
+        <v>1778.2094800499999</v>
       </c>
       <c r="F101" t="s">
         <v>175</v>
@@ -15912,13 +15923,13 @@
         <v>8</v>
       </c>
       <c r="C102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D102">
         <v>4</v>
       </c>
       <c r="E102" s="81">
-        <v>1777.12373996</v>
+        <v>1767.6294798900001</v>
       </c>
       <c r="F102" t="s">
         <v>175</v>
@@ -15932,16 +15943,13 @@
         <v>8</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D103">
         <v>4</v>
       </c>
       <c r="E103" s="81">
-        <v>1777.3397109499999</v>
-      </c>
-      <c r="F103" t="s">
-        <v>175</v>
+        <v>1755.7615511399999</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -15952,16 +15960,13 @@
         <v>8</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D104">
         <v>4</v>
       </c>
       <c r="E104" s="81">
-        <v>1770.9294168900001</v>
-      </c>
-      <c r="F104" t="s">
-        <v>175</v>
+        <v>1755.3108708899999</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -15972,16 +15977,13 @@
         <v>8</v>
       </c>
       <c r="C105">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D105">
         <v>4</v>
       </c>
       <c r="E105" s="81">
-        <v>1827.6398251099999</v>
-      </c>
-      <c r="F105" t="s">
-        <v>175</v>
+        <v>1776.3025808299999</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -15992,16 +15994,13 @@
         <v>8</v>
       </c>
       <c r="C106">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D106">
         <v>4</v>
       </c>
       <c r="E106" s="81">
-        <v>1673.44356012</v>
-      </c>
-      <c r="F106" t="s">
-        <v>175</v>
+        <v>1775.4375519800001</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -16012,16 +16011,13 @@
         <v>8</v>
       </c>
       <c r="C107">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D107">
         <v>4</v>
       </c>
       <c r="E107" s="81">
-        <v>1804.07670403</v>
-      </c>
-      <c r="F107" t="s">
-        <v>175</v>
+        <v>1771.63202095</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -16032,13 +16028,13 @@
         <v>8</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D108">
         <v>4</v>
       </c>
       <c r="E108" s="81">
-        <v>1803.94324398</v>
+        <v>1727.25121689</v>
       </c>
       <c r="F108" t="s">
         <v>175</v>
@@ -16052,13 +16048,13 @@
         <v>8</v>
       </c>
       <c r="C109">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D109">
         <v>4</v>
       </c>
       <c r="E109" s="81">
-        <v>1806.8634729400001</v>
+        <v>1818.3420629499999</v>
       </c>
       <c r="F109" t="s">
         <v>175</v>
@@ -16072,13 +16068,13 @@
         <v>8</v>
       </c>
       <c r="C110">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D110">
         <v>4</v>
       </c>
       <c r="E110" s="81">
-        <v>1810.6687281100001</v>
+        <v>1770.4413349599999</v>
       </c>
       <c r="F110" t="s">
         <v>175</v>
@@ -16092,13 +16088,13 @@
         <v>8</v>
       </c>
       <c r="C111">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D111">
         <v>4</v>
       </c>
       <c r="E111" s="81">
-        <v>1781.2703998100001</v>
+        <v>1894.0333972000001</v>
       </c>
       <c r="F111" t="s">
         <v>175</v>
@@ -16112,13 +16108,13 @@
         <v>8</v>
       </c>
       <c r="C112">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D112">
         <v>4</v>
       </c>
       <c r="E112" s="81">
-        <v>1815.0974919800001</v>
+        <v>1777.12373996</v>
       </c>
       <c r="F112" t="s">
         <v>175</v>
@@ -16132,13 +16128,13 @@
         <v>8</v>
       </c>
       <c r="C113">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D113">
         <v>4</v>
       </c>
       <c r="E113" s="81">
-        <v>1888.6297318899999</v>
+        <v>1777.3397109499999</v>
       </c>
       <c r="F113" t="s">
         <v>175</v>
@@ -16152,13 +16148,13 @@
         <v>8</v>
       </c>
       <c r="C114">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D114">
         <v>4</v>
       </c>
       <c r="E114" s="81">
-        <v>1798.8409340400001</v>
+        <v>1770.9294168900001</v>
       </c>
       <c r="F114" t="s">
         <v>175</v>
@@ -16178,7 +16174,7 @@
         <v>4</v>
       </c>
       <c r="E115" s="81">
-        <v>1800.7364668800001</v>
+        <v>1827.6398251099999</v>
       </c>
       <c r="F115" t="s">
         <v>175</v>
@@ -16198,7 +16194,7 @@
         <v>4</v>
       </c>
       <c r="E116" s="81">
-        <v>1777.75735998</v>
+        <v>1673.44356012</v>
       </c>
       <c r="F116" t="s">
         <v>175</v>
@@ -16218,7 +16214,7 @@
         <v>4</v>
       </c>
       <c r="E117" s="81">
-        <v>1790.2442941700001</v>
+        <v>1804.07670403</v>
       </c>
       <c r="F117" t="s">
         <v>175</v>
@@ -16238,7 +16234,7 @@
         <v>4</v>
       </c>
       <c r="E118" s="81">
-        <v>1921.4787900399999</v>
+        <v>1803.94324398</v>
       </c>
       <c r="F118" t="s">
         <v>175</v>
@@ -16258,7 +16254,7 @@
         <v>4</v>
       </c>
       <c r="E119" s="81">
-        <v>1807.1237280400001</v>
+        <v>1806.8634729400001</v>
       </c>
       <c r="F119" t="s">
         <v>175</v>
@@ -16278,7 +16274,7 @@
         <v>4</v>
       </c>
       <c r="E120" s="81">
-        <v>1918.3057050699999</v>
+        <v>1810.6687281100001</v>
       </c>
       <c r="F120" t="s">
         <v>175</v>
@@ -16298,7 +16294,7 @@
         <v>4</v>
       </c>
       <c r="E121" s="81">
-        <v>1782.99450207</v>
+        <v>1781.2703998100001</v>
       </c>
       <c r="F121" t="s">
         <v>175</v>
@@ -16318,7 +16314,7 @@
         <v>4</v>
       </c>
       <c r="E122" s="81">
-        <v>1789.0848701</v>
+        <v>1815.0974919800001</v>
       </c>
       <c r="F122" t="s">
         <v>175</v>
@@ -16338,7 +16334,7 @@
         <v>4</v>
       </c>
       <c r="E123" s="81">
-        <v>1712.9129622</v>
+        <v>1888.6297318899999</v>
       </c>
       <c r="F123" t="s">
         <v>175</v>
@@ -16358,7 +16354,7 @@
         <v>4</v>
       </c>
       <c r="E124" s="81">
-        <v>1810.1466629500001</v>
+        <v>1798.8409340400001</v>
       </c>
       <c r="F124" t="s">
         <v>175</v>
@@ -16378,29 +16374,29 @@
         <v>4</v>
       </c>
       <c r="E125" s="81">
-        <v>1818.4292981599999</v>
+        <v>1800.7364668800001</v>
       </c>
       <c r="F125" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="72" t="s">
+      <c r="A126" t="s">
         <v>177</v>
       </c>
-      <c r="B126" s="72">
-        <v>8</v>
-      </c>
-      <c r="C126" s="72">
-        <v>16</v>
-      </c>
-      <c r="D126" s="72">
-        <v>4</v>
-      </c>
-      <c r="E126" s="83">
-        <v>1842.58875704</v>
-      </c>
-      <c r="F126" s="72" t="s">
+      <c r="B126">
+        <v>8</v>
+      </c>
+      <c r="C126">
+        <v>8</v>
+      </c>
+      <c r="D126">
+        <v>4</v>
+      </c>
+      <c r="E126" s="81">
+        <v>1777.75735998</v>
+      </c>
+      <c r="F126" t="s">
         <v>175</v>
       </c>
     </row>
@@ -16408,17 +16404,17 @@
       <c r="A127" t="s">
         <v>177</v>
       </c>
-      <c r="B127" s="47">
-        <v>8</v>
-      </c>
-      <c r="C127" s="47">
-        <v>16</v>
-      </c>
-      <c r="D127" s="47">
+      <c r="B127">
+        <v>8</v>
+      </c>
+      <c r="C127">
+        <v>8</v>
+      </c>
+      <c r="D127">
         <v>4</v>
       </c>
       <c r="E127" s="81">
-        <v>1835.8984041199999</v>
+        <v>1790.2442941700001</v>
       </c>
       <c r="F127" t="s">
         <v>175</v>
@@ -16428,17 +16424,17 @@
       <c r="A128" t="s">
         <v>177</v>
       </c>
-      <c r="B128" s="47">
-        <v>8</v>
-      </c>
-      <c r="C128" s="47">
-        <v>16</v>
-      </c>
-      <c r="D128" s="47">
+      <c r="B128">
+        <v>8</v>
+      </c>
+      <c r="C128">
+        <v>8</v>
+      </c>
+      <c r="D128">
         <v>4</v>
       </c>
       <c r="E128" s="81">
-        <v>1715.9458088900001</v>
+        <v>1921.4787900399999</v>
       </c>
       <c r="F128" t="s">
         <v>175</v>
@@ -16448,17 +16444,17 @@
       <c r="A129" t="s">
         <v>177</v>
       </c>
-      <c r="B129" s="47">
-        <v>8</v>
-      </c>
-      <c r="C129" s="47">
-        <v>16</v>
-      </c>
-      <c r="D129" s="47">
+      <c r="B129">
+        <v>8</v>
+      </c>
+      <c r="C129">
+        <v>8</v>
+      </c>
+      <c r="D129">
         <v>4</v>
       </c>
       <c r="E129" s="81">
-        <v>1759.9219129099999</v>
+        <v>1807.1237280400001</v>
       </c>
       <c r="F129" t="s">
         <v>175</v>
@@ -16468,17 +16464,17 @@
       <c r="A130" t="s">
         <v>177</v>
       </c>
-      <c r="B130" s="47">
-        <v>8</v>
-      </c>
-      <c r="C130" s="47">
-        <v>16</v>
-      </c>
-      <c r="D130" s="47">
+      <c r="B130">
+        <v>8</v>
+      </c>
+      <c r="C130">
+        <v>8</v>
+      </c>
+      <c r="D130">
         <v>4</v>
       </c>
       <c r="E130" s="81">
-        <v>1836.24597597</v>
+        <v>1918.3057050699999</v>
       </c>
       <c r="F130" t="s">
         <v>175</v>
@@ -16488,17 +16484,17 @@
       <c r="A131" t="s">
         <v>177</v>
       </c>
-      <c r="B131" s="47">
-        <v>8</v>
-      </c>
-      <c r="C131" s="47">
-        <v>16</v>
-      </c>
-      <c r="D131" s="47">
+      <c r="B131">
+        <v>8</v>
+      </c>
+      <c r="C131">
+        <v>8</v>
+      </c>
+      <c r="D131">
         <v>4</v>
       </c>
       <c r="E131" s="81">
-        <v>1839.4019022</v>
+        <v>1782.99450207</v>
       </c>
       <c r="F131" t="s">
         <v>175</v>
@@ -16508,17 +16504,17 @@
       <c r="A132" t="s">
         <v>177</v>
       </c>
-      <c r="B132" s="47">
-        <v>8</v>
-      </c>
-      <c r="C132" s="47">
-        <v>16</v>
-      </c>
-      <c r="D132" s="47">
+      <c r="B132">
+        <v>8</v>
+      </c>
+      <c r="C132">
+        <v>8</v>
+      </c>
+      <c r="D132">
         <v>4</v>
       </c>
       <c r="E132" s="81">
-        <v>1706.54768085</v>
+        <v>1789.0848701</v>
       </c>
       <c r="F132" t="s">
         <v>175</v>
@@ -16528,17 +16524,17 @@
       <c r="A133" t="s">
         <v>177</v>
       </c>
-      <c r="B133" s="47">
-        <v>8</v>
-      </c>
-      <c r="C133" s="47">
-        <v>16</v>
-      </c>
-      <c r="D133" s="47">
+      <c r="B133">
+        <v>8</v>
+      </c>
+      <c r="C133">
+        <v>8</v>
+      </c>
+      <c r="D133">
         <v>4</v>
       </c>
       <c r="E133" s="81">
-        <v>1824.0260689300001</v>
+        <v>1712.9129622</v>
       </c>
       <c r="F133" t="s">
         <v>175</v>
@@ -16548,17 +16544,17 @@
       <c r="A134" t="s">
         <v>177</v>
       </c>
-      <c r="B134" s="47">
-        <v>8</v>
-      </c>
-      <c r="C134" s="47">
-        <v>16</v>
-      </c>
-      <c r="D134" s="47">
+      <c r="B134">
+        <v>8</v>
+      </c>
+      <c r="C134">
+        <v>8</v>
+      </c>
+      <c r="D134">
         <v>4</v>
       </c>
       <c r="E134" s="81">
-        <v>1812.6436419500001</v>
+        <v>1810.1466629500001</v>
       </c>
       <c r="F134" t="s">
         <v>175</v>
@@ -16566,59 +16562,59 @@
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B135">
         <v>8</v>
       </c>
       <c r="C135">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D135">
         <v>4</v>
       </c>
       <c r="E135" s="81">
-        <v>1658.3445510900001</v>
+        <v>1818.4292981599999</v>
       </c>
       <c r="F135" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="136" spans="1:6">
-      <c r="A136" t="s">
-        <v>176</v>
-      </c>
-      <c r="B136">
-        <v>8</v>
-      </c>
-      <c r="C136">
-        <v>32</v>
-      </c>
-      <c r="D136">
-        <v>4</v>
-      </c>
-      <c r="E136" s="81">
-        <v>1720.03288198</v>
-      </c>
-      <c r="F136" t="s">
+      <c r="A136" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B136" s="72">
+        <v>8</v>
+      </c>
+      <c r="C136" s="72">
+        <v>16</v>
+      </c>
+      <c r="D136" s="72">
+        <v>4</v>
+      </c>
+      <c r="E136" s="83">
+        <v>1842.58875704</v>
+      </c>
+      <c r="F136" s="72" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>176</v>
-      </c>
-      <c r="B137">
-        <v>8</v>
-      </c>
-      <c r="C137">
-        <v>32</v>
-      </c>
-      <c r="D137">
+        <v>177</v>
+      </c>
+      <c r="B137" s="47">
+        <v>8</v>
+      </c>
+      <c r="C137" s="47">
+        <v>16</v>
+      </c>
+      <c r="D137" s="47">
         <v>4</v>
       </c>
       <c r="E137" s="81">
-        <v>1711.9533910800001</v>
+        <v>1835.8984041199999</v>
       </c>
       <c r="F137" t="s">
         <v>175</v>
@@ -16626,19 +16622,19 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>176</v>
-      </c>
-      <c r="B138">
-        <v>8</v>
-      </c>
-      <c r="C138">
-        <v>32</v>
-      </c>
-      <c r="D138">
+        <v>177</v>
+      </c>
+      <c r="B138" s="47">
+        <v>8</v>
+      </c>
+      <c r="C138" s="47">
+        <v>16</v>
+      </c>
+      <c r="D138" s="47">
         <v>4</v>
       </c>
       <c r="E138" s="81">
-        <v>1668.2077360200001</v>
+        <v>1715.9458088900001</v>
       </c>
       <c r="F138" t="s">
         <v>175</v>
@@ -16646,279 +16642,972 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>176</v>
-      </c>
-      <c r="B139">
-        <v>8</v>
-      </c>
-      <c r="C139">
-        <v>32</v>
-      </c>
-      <c r="D139">
+        <v>177</v>
+      </c>
+      <c r="B139" s="47">
+        <v>8</v>
+      </c>
+      <c r="C139" s="47">
+        <v>16</v>
+      </c>
+      <c r="D139" s="47">
         <v>4</v>
       </c>
       <c r="E139" s="81">
-        <v>1698.93364692</v>
+        <v>1759.9219129099999</v>
       </c>
       <c r="F139" t="s">
         <v>175</v>
       </c>
     </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>177</v>
+      </c>
+      <c r="B140" s="47">
+        <v>8</v>
+      </c>
+      <c r="C140" s="47">
+        <v>16</v>
+      </c>
+      <c r="D140" s="47">
+        <v>4</v>
+      </c>
+      <c r="E140" s="81">
+        <v>1836.24597597</v>
+      </c>
+      <c r="F140" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>177</v>
+      </c>
+      <c r="B141" s="47">
+        <v>8</v>
+      </c>
+      <c r="C141" s="47">
+        <v>16</v>
+      </c>
+      <c r="D141" s="47">
+        <v>4</v>
+      </c>
+      <c r="E141" s="81">
+        <v>1839.4019022</v>
+      </c>
+      <c r="F141" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>177</v>
+      </c>
+      <c r="B142" s="47">
+        <v>8</v>
+      </c>
+      <c r="C142" s="47">
+        <v>16</v>
+      </c>
+      <c r="D142" s="47">
+        <v>4</v>
+      </c>
+      <c r="E142" s="81">
+        <v>1706.54768085</v>
+      </c>
+      <c r="F142" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>177</v>
+      </c>
+      <c r="B143" s="47">
+        <v>8</v>
+      </c>
+      <c r="C143" s="47">
+        <v>16</v>
+      </c>
+      <c r="D143" s="47">
+        <v>4</v>
+      </c>
+      <c r="E143" s="81">
+        <v>1824.0260689300001</v>
+      </c>
+      <c r="F143" t="s">
+        <v>175</v>
+      </c>
+    </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
+        <v>177</v>
+      </c>
+      <c r="B144" s="47">
+        <v>8</v>
+      </c>
+      <c r="C144" s="47">
+        <v>16</v>
+      </c>
+      <c r="D144" s="47">
+        <v>4</v>
+      </c>
+      <c r="E144" s="81">
+        <v>1812.6436419500001</v>
+      </c>
+      <c r="F144" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>176</v>
+      </c>
+      <c r="B145">
+        <v>8</v>
+      </c>
+      <c r="C145">
+        <v>32</v>
+      </c>
+      <c r="D145">
+        <v>4</v>
+      </c>
+      <c r="E145" s="81">
+        <v>1658.3445510900001</v>
+      </c>
+      <c r="F145" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>176</v>
+      </c>
+      <c r="B146">
+        <v>8</v>
+      </c>
+      <c r="C146">
+        <v>32</v>
+      </c>
+      <c r="D146">
+        <v>4</v>
+      </c>
+      <c r="E146" s="81">
+        <v>1720.03288198</v>
+      </c>
+      <c r="F146" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>176</v>
+      </c>
+      <c r="B147">
+        <v>8</v>
+      </c>
+      <c r="C147">
+        <v>32</v>
+      </c>
+      <c r="D147">
+        <v>4</v>
+      </c>
+      <c r="E147" s="81">
+        <v>1711.9533910800001</v>
+      </c>
+      <c r="F147" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>176</v>
+      </c>
+      <c r="B148">
+        <v>8</v>
+      </c>
+      <c r="C148">
+        <v>32</v>
+      </c>
+      <c r="D148">
+        <v>4</v>
+      </c>
+      <c r="E148" s="81">
+        <v>1668.2077360200001</v>
+      </c>
+      <c r="F148" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>176</v>
+      </c>
+      <c r="B149">
+        <v>8</v>
+      </c>
+      <c r="C149">
+        <v>32</v>
+      </c>
+      <c r="D149">
+        <v>4</v>
+      </c>
+      <c r="E149" s="81">
+        <v>1698.93364692</v>
+      </c>
+      <c r="F149" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
-      <c r="A145" t="s">
+    <row r="155" spans="1:6">
+      <c r="A155" t="s">
         <v>9</v>
-      </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-      <c r="C145">
-        <v>2</v>
-      </c>
-      <c r="D145">
-        <v>4</v>
-      </c>
-      <c r="E145">
-        <v>5144.30550408</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" t="s">
-        <v>9</v>
-      </c>
-      <c r="B146">
-        <v>1</v>
-      </c>
-      <c r="C146">
-        <v>2</v>
-      </c>
-      <c r="D146">
-        <v>4</v>
-      </c>
-      <c r="E146">
-        <v>5111.4611360999997</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" t="s">
-        <v>9</v>
-      </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-      <c r="C147">
-        <v>2</v>
-      </c>
-      <c r="D147">
-        <v>4</v>
-      </c>
-      <c r="E147">
-        <v>5201.5161449899997</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="A148" t="s">
-        <v>9</v>
-      </c>
-      <c r="B148">
-        <v>1</v>
-      </c>
-      <c r="C148">
-        <v>4</v>
-      </c>
-      <c r="D148">
-        <v>4</v>
-      </c>
-      <c r="E148">
-        <v>5209.3013448700003</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="A149" t="s">
-        <v>9</v>
-      </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-      <c r="C149">
-        <v>4</v>
-      </c>
-      <c r="D149">
-        <v>4</v>
-      </c>
-      <c r="E149">
-        <v>5101.5123591399997</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="A150" t="s">
-        <v>9</v>
-      </c>
-      <c r="B150">
-        <v>1</v>
-      </c>
-      <c r="C150">
-        <v>4</v>
-      </c>
-      <c r="D150">
-        <v>4</v>
-      </c>
-      <c r="E150">
-        <v>5179.61960602</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="A151" t="s">
-        <v>8</v>
-      </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
-      <c r="C151">
-        <v>8</v>
-      </c>
-      <c r="D151">
-        <v>4</v>
-      </c>
-      <c r="E151">
-        <v>5135.1033690000004</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="A152" t="s">
-        <v>8</v>
-      </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-      <c r="C152">
-        <v>8</v>
-      </c>
-      <c r="D152">
-        <v>4</v>
-      </c>
-      <c r="E152">
-        <v>5158.3376369999996</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
-      <c r="A153" t="s">
-        <v>8</v>
-      </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
-      <c r="C153">
-        <v>8</v>
-      </c>
-      <c r="D153">
-        <v>4</v>
-      </c>
-      <c r="E153">
-        <v>5240.7737269999998</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="A154" t="s">
-        <v>8</v>
-      </c>
-      <c r="B154">
-        <v>1</v>
-      </c>
-      <c r="C154">
-        <v>16</v>
-      </c>
-      <c r="D154">
-        <v>4</v>
-      </c>
-      <c r="E154">
-        <v>5207.7800388300002</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="A155" t="s">
-        <v>8</v>
       </c>
       <c r="B155">
         <v>1</v>
       </c>
       <c r="C155">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D155">
         <v>4</v>
       </c>
       <c r="E155">
-        <v>5193.0061578799996</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+        <v>5144.30550408</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B156">
         <v>1</v>
       </c>
       <c r="C156">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D156">
         <v>4</v>
       </c>
       <c r="E156">
-        <v>5216.1367888499999</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+        <v>5111.4611360999997</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B157">
         <v>1</v>
       </c>
       <c r="C157">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D157">
         <v>4</v>
       </c>
       <c r="E157">
-        <v>5382.3301620000002</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+        <v>5201.5161449899997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B158">
         <v>1</v>
       </c>
       <c r="C158">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D158">
         <v>4</v>
       </c>
       <c r="E158">
-        <v>5421.3847939999996</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
+        <v>5209.3013448700003</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B159">
         <v>1</v>
       </c>
       <c r="C159">
+        <v>4</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+      <c r="E159">
+        <v>5101.5123591399997</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>4</v>
+      </c>
+      <c r="D160">
+        <v>4</v>
+      </c>
+      <c r="E160">
+        <v>5179.61960602</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>8</v>
+      </c>
+      <c r="D161">
+        <v>4</v>
+      </c>
+      <c r="E161">
+        <v>5135.1033690000004</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>8</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>8</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+      <c r="E162">
+        <v>5158.3376369999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>8</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>8</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+      <c r="E163">
+        <v>5240.7737269999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>16</v>
+      </c>
+      <c r="D164">
+        <v>4</v>
+      </c>
+      <c r="E164">
+        <v>5207.7800388300002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>16</v>
+      </c>
+      <c r="D165">
+        <v>4</v>
+      </c>
+      <c r="E165">
+        <v>5193.0061578799996</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>8</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>16</v>
+      </c>
+      <c r="D166">
+        <v>4</v>
+      </c>
+      <c r="E166">
+        <v>5216.1367888499999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="C167">
         <v>32</v>
       </c>
-      <c r="D159">
-        <v>4</v>
+      <c r="D167">
+        <v>4</v>
+      </c>
+      <c r="E167">
+        <v>5382.3301620000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="C168">
+        <v>32</v>
+      </c>
+      <c r="D168">
+        <v>4</v>
+      </c>
+      <c r="E168">
+        <v>5421.3847939999996</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
+      <c r="C169">
+        <v>32</v>
+      </c>
+      <c r="D169">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B171" s="74">
+        <v>4</v>
+      </c>
+      <c r="C171" s="74">
+        <v>2</v>
+      </c>
+      <c r="D171" s="74">
+        <v>4</v>
+      </c>
+      <c r="E171">
+        <v>2165.2144379599999</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B172" s="74">
+        <v>4</v>
+      </c>
+      <c r="C172" s="74">
+        <v>2</v>
+      </c>
+      <c r="D172" s="74">
+        <v>4</v>
+      </c>
+      <c r="E172">
+        <v>2283.2516999200002</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="74">
+        <v>4</v>
+      </c>
+      <c r="C173" s="74">
+        <v>2</v>
+      </c>
+      <c r="D173" s="74">
+        <v>4</v>
+      </c>
+      <c r="E173">
+        <v>2173.3167338399999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B174" s="74">
+        <v>4</v>
+      </c>
+      <c r="C174" s="74">
+        <v>2</v>
+      </c>
+      <c r="D174" s="74">
+        <v>4</v>
+      </c>
+      <c r="E174">
+        <v>2185.1247549099999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B175" s="74">
+        <v>4</v>
+      </c>
+      <c r="C175" s="74">
+        <v>2</v>
+      </c>
+      <c r="D175" s="74">
+        <v>4</v>
+      </c>
+      <c r="E175">
+        <v>2269.9999311000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="74">
+        <v>4</v>
+      </c>
+      <c r="C176" s="74">
+        <v>2</v>
+      </c>
+      <c r="D176" s="74">
+        <v>4</v>
+      </c>
+      <c r="E176">
+        <v>2162.0369491599999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B177" s="74">
+        <v>4</v>
+      </c>
+      <c r="C177" s="74">
+        <v>4</v>
+      </c>
+      <c r="D177" s="74">
+        <v>4</v>
+      </c>
+      <c r="E177">
+        <v>2319.98405099</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B178" s="74">
+        <v>4</v>
+      </c>
+      <c r="C178" s="74">
+        <v>4</v>
+      </c>
+      <c r="D178" s="74">
+        <v>4</v>
+      </c>
+      <c r="E178">
+        <v>2165.4693579700001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B179" s="74">
+        <v>4</v>
+      </c>
+      <c r="C179" s="74">
+        <v>4</v>
+      </c>
+      <c r="D179" s="74">
+        <v>4</v>
+      </c>
+      <c r="E179">
+        <v>2171.7986049699998</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B180" s="74">
+        <v>4</v>
+      </c>
+      <c r="C180" s="74">
+        <v>4</v>
+      </c>
+      <c r="D180" s="74">
+        <v>4</v>
+      </c>
+      <c r="E180">
+        <v>2183.7792851899999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B181" s="74">
+        <v>4</v>
+      </c>
+      <c r="C181" s="74">
+        <v>4</v>
+      </c>
+      <c r="D181" s="74">
+        <v>4</v>
+      </c>
+      <c r="E181">
+        <v>2185.2494609400001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B182" s="74">
+        <v>4</v>
+      </c>
+      <c r="C182" s="74">
+        <v>8</v>
+      </c>
+      <c r="D182" s="74">
+        <v>4</v>
+      </c>
+      <c r="E182">
+        <v>2137.2723250399999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B183" s="74">
+        <v>4</v>
+      </c>
+      <c r="C183" s="74">
+        <v>8</v>
+      </c>
+      <c r="D183" s="74">
+        <v>4</v>
+      </c>
+      <c r="E183">
+        <v>2220.7439541799999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B184" s="74">
+        <v>4</v>
+      </c>
+      <c r="C184" s="74">
+        <v>8</v>
+      </c>
+      <c r="D184" s="74">
+        <v>4</v>
+      </c>
+      <c r="E184">
+        <v>2110.8885998699998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B185" s="74">
+        <v>4</v>
+      </c>
+      <c r="C185" s="74">
+        <v>8</v>
+      </c>
+      <c r="D185" s="74">
+        <v>4</v>
+      </c>
+      <c r="E185">
+        <v>2212.8257401000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B186" s="74">
+        <v>4</v>
+      </c>
+      <c r="C186" s="74">
+        <v>8</v>
+      </c>
+      <c r="D186" s="74">
+        <v>4</v>
+      </c>
+      <c r="E186">
+        <v>2209.1583819399998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B187" s="74">
+        <v>4</v>
+      </c>
+      <c r="C187" s="74">
+        <v>8</v>
+      </c>
+      <c r="D187" s="74">
+        <v>4</v>
+      </c>
+      <c r="E187">
+        <v>2225.3706951099998</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B188" s="74">
+        <v>4</v>
+      </c>
+      <c r="C188" s="74">
+        <v>16</v>
+      </c>
+      <c r="D188" s="74">
+        <v>4</v>
+      </c>
+      <c r="E188">
+        <v>2225.0072731999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B189" s="74">
+        <v>4</v>
+      </c>
+      <c r="C189" s="74">
+        <v>16</v>
+      </c>
+      <c r="D189" s="74">
+        <v>4</v>
+      </c>
+      <c r="E189">
+        <v>2296.1518640499999</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B190" s="74">
+        <v>4</v>
+      </c>
+      <c r="C190" s="74">
+        <v>16</v>
+      </c>
+      <c r="D190" s="74">
+        <v>4</v>
+      </c>
+      <c r="E190">
+        <v>2285.0504000199999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B191" s="74">
+        <v>4</v>
+      </c>
+      <c r="C191" s="74">
+        <v>16</v>
+      </c>
+      <c r="D191" s="74">
+        <v>4</v>
+      </c>
+      <c r="E191">
+        <v>2199.4940891299998</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B192" s="74">
+        <v>4</v>
+      </c>
+      <c r="C192" s="74">
+        <v>16</v>
+      </c>
+      <c r="D192" s="74">
+        <v>4</v>
+      </c>
+      <c r="E192">
+        <v>2291.9013450100001</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B193" s="74">
+        <v>4</v>
+      </c>
+      <c r="C193" s="74">
+        <v>16</v>
+      </c>
+      <c r="D193" s="74">
+        <v>4</v>
+      </c>
+      <c r="E193">
+        <v>2299.9718630299999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B194" s="74">
+        <v>4</v>
+      </c>
+      <c r="C194" s="74">
+        <v>32</v>
+      </c>
+      <c r="D194" s="74">
+        <v>4</v>
+      </c>
+      <c r="E194">
+        <v>3112.5267729799998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B195" s="74">
+        <v>4</v>
+      </c>
+      <c r="C195" s="74">
+        <v>32</v>
+      </c>
+      <c r="D195" s="74">
+        <v>4</v>
+      </c>
+      <c r="E195">
+        <v>3114.49228692</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B196" s="74">
+        <v>4</v>
+      </c>
+      <c r="C196" s="74">
+        <v>32</v>
+      </c>
+      <c r="D196" s="74">
+        <v>4</v>
+      </c>
+      <c r="E196">
+        <v>2319.8565950399998</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B197" s="74">
+        <v>4</v>
+      </c>
+      <c r="C197" s="74">
+        <v>32</v>
+      </c>
+      <c r="D197" s="74">
+        <v>4</v>
+      </c>
+      <c r="E197">
+        <v>2326.5095250600002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B198" s="74">
+        <v>4</v>
+      </c>
+      <c r="C198" s="74">
+        <v>32</v>
+      </c>
+      <c r="D198" s="74">
+        <v>4</v>
+      </c>
+      <c r="E198">
+        <v>3192.1907022</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B199" s="74">
+        <v>4</v>
+      </c>
+      <c r="C199" s="74">
+        <v>32</v>
+      </c>
+      <c r="D199" s="74">
+        <v>4</v>
+      </c>
+      <c r="E199">
+        <v>2289.49348998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>